<commit_message>
Add info on runner-up in spreadsheet.
</commit_message>
<xml_diff>
--- a/valgresultat_2019_lillestrom.xlsx
+++ b/valgresultat_2019_lillestrom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C7BB8F-EE75-4F3A-98AB-D94D858230E5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3052EA-D3B9-48C5-86AE-588C6133254C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="2" xr2:uid="{A5AA8802-A06A-47C3-A471-EB2F0168D772}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
   <si>
     <t>Mottatte forhåndstemmegivninger</t>
   </si>
@@ -259,13 +259,22 @@
   </si>
   <si>
     <t>Mandater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                             (56)</t>
+  </si>
+  <si>
+    <t>Runner-up</t>
+  </si>
+  <si>
+    <t>(Ap)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +314,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -354,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -372,6 +388,9 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1338,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6A3DFA-BBE1-474B-A1F8-0F3A1E625FD4}">
   <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2154,6 +2173,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A60" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60" s="16">
+        <v>19646.969696969696</v>
+      </c>
+      <c r="F60" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>70</v>
@@ -3353,7 +3386,7 @@
       <c r="C81">
         <v>33</v>
       </c>
-      <c r="D81" s="14">
+      <c r="D81" s="15">
         <f t="shared" si="6"/>
         <v>19646.969696969696</v>
       </c>

</xml_diff>